<commit_message>
Cập nhật file Tasks
</commit_message>
<xml_diff>
--- a/BC-Capstone-Bootstrap-Tasks.xlsx
+++ b/BC-Capstone-Bootstrap-Tasks.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LEARNING-Cybersoft\3.BOOTSTRAP\Bai lam\BC-Capstone-Bootstrap-Pooch-Care\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59EA8D1-F47E-4B85-98E0-28F4D91886EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -193,38 +202,38 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF363636"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -234,7 +243,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -274,31 +283,12 @@
     </fill>
   </fills>
   <borders count="5">
-    <border/>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -307,76 +297,100 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="9" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="9" fontId="5" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="6" fontId="4" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="7" fontId="5" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -566,20 +580,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -612,7 +631,7 @@
       </c>
       <c r="K1" s="6"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -623,7 +642,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="9">
-        <v>0.0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>12</v>
@@ -635,7 +654,7 @@
         <v>14</v>
       </c>
       <c r="H2" s="11">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>15</v>
@@ -643,7 +662,7 @@
       <c r="J2" s="12"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
@@ -654,7 +673,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="9">
-        <v>0.0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>12</v>
@@ -666,7 +685,7 @@
         <v>19</v>
       </c>
       <c r="H3" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I3" s="10" t="s">
         <v>15</v>
@@ -674,7 +693,7 @@
       <c r="J3" s="12"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
@@ -685,7 +704,7 @@
         <v>21</v>
       </c>
       <c r="D4" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>22</v>
@@ -697,7 +716,7 @@
         <v>24</v>
       </c>
       <c r="H4" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I4" s="10" t="s">
         <v>12</v>
@@ -705,7 +724,7 @@
       <c r="J4" s="12"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>25</v>
       </c>
@@ -716,7 +735,7 @@
         <v>26</v>
       </c>
       <c r="D5" s="9">
-        <v>0.0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>15</v>
@@ -728,7 +747,7 @@
         <v>28</v>
       </c>
       <c r="H5" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>22</v>
@@ -736,7 +755,7 @@
       <c r="J5" s="12"/>
       <c r="K5" s="6"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>29</v>
       </c>
@@ -747,7 +766,7 @@
         <v>30</v>
       </c>
       <c r="D6" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>22</v>
@@ -759,7 +778,7 @@
         <v>32</v>
       </c>
       <c r="H6" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I6" s="10" t="s">
         <v>12</v>
@@ -767,7 +786,7 @@
       <c r="J6" s="12"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>33</v>
       </c>
@@ -778,7 +797,7 @@
         <v>34</v>
       </c>
       <c r="D7" s="9">
-        <v>0.0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>15</v>
@@ -790,7 +809,7 @@
         <v>36</v>
       </c>
       <c r="H7" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>22</v>
@@ -798,7 +817,7 @@
       <c r="J7" s="12"/>
       <c r="K7" s="6"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>37</v>
       </c>
@@ -809,7 +828,7 @@
         <v>38</v>
       </c>
       <c r="D8" s="9">
-        <v>0.0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>12</v>
@@ -821,7 +840,7 @@
         <v>40</v>
       </c>
       <c r="H8" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I8" s="10" t="s">
         <v>15</v>
@@ -829,7 +848,7 @@
       <c r="J8" s="12"/>
       <c r="K8" s="6"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>41</v>
       </c>
@@ -840,7 +859,7 @@
         <v>42</v>
       </c>
       <c r="D9" s="9">
-        <v>0.0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>15</v>
@@ -852,7 +871,7 @@
         <v>44</v>
       </c>
       <c r="H9" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>22</v>
@@ -860,7 +879,7 @@
       <c r="J9" s="12"/>
       <c r="K9" s="6"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -871,7 +890,7 @@
         <v>46</v>
       </c>
       <c r="D10" s="9">
-        <v>0.0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>15</v>
@@ -883,7 +902,7 @@
         <v>48</v>
       </c>
       <c r="H10" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I10" s="10" t="s">
         <v>22</v>
@@ -891,7 +910,7 @@
       <c r="J10" s="12"/>
       <c r="K10" s="6"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>49</v>
       </c>
@@ -902,7 +921,7 @@
         <v>50</v>
       </c>
       <c r="D11" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>22</v>
@@ -914,7 +933,7 @@
         <v>52</v>
       </c>
       <c r="H11" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I11" s="10" t="s">
         <v>12</v>
@@ -922,7 +941,7 @@
       <c r="J11" s="12"/>
       <c r="K11" s="6"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>53</v>
       </c>
@@ -933,7 +952,7 @@
         <v>54</v>
       </c>
       <c r="D12" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>22</v>
@@ -945,7 +964,7 @@
         <v>56</v>
       </c>
       <c r="H12" s="9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>12</v>
@@ -954,6 +973,6 @@
       <c r="K12" s="6"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cập nhật giao diện hoàn chỉnh
</commit_message>
<xml_diff>
--- a/BC-Capstone-Bootstrap-Tasks.xlsx
+++ b/BC-Capstone-Bootstrap-Tasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\BC-Capstone-Bootstrap-Pooch-Care\BC-Capstone-Bootstrap-Pooch-Care\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LEARNING-Cybersoft\3.BOOTSTRAP\Bai lam\BC-Capstone-Bootstrap-Pooch-Care\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C2879B-A52C-49CC-A451-1B41568D95FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE8DDD8-72EE-4696-ACB2-546CAAFCFE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -238,7 +238,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -275,12 +275,6 @@
         <bgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFAEABAB"/>
-        <bgColor rgb="FFAEABAB"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -346,19 +340,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -368,10 +362,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,12 +584,12 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -631,7 +622,7 @@
       </c>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -653,16 +644,16 @@
       <c r="G2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="11">
-        <v>0</v>
+      <c r="H2" s="9">
+        <v>1</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="12"/>
+      <c r="J2" s="11"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
@@ -685,15 +676,15 @@
         <v>19</v>
       </c>
       <c r="H3" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="12"/>
+      <c r="J3" s="11"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
@@ -704,7 +695,7 @@
         <v>21</v>
       </c>
       <c r="D4" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>22</v>
@@ -716,15 +707,15 @@
         <v>24</v>
       </c>
       <c r="H4" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="12"/>
+      <c r="J4" s="11"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>25</v>
       </c>
@@ -735,7 +726,7 @@
         <v>26</v>
       </c>
       <c r="D5" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>15</v>
@@ -747,15 +738,15 @@
         <v>28</v>
       </c>
       <c r="H5" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="12"/>
+      <c r="J5" s="11"/>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>29</v>
       </c>
@@ -766,7 +757,7 @@
         <v>30</v>
       </c>
       <c r="D6" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>22</v>
@@ -778,15 +769,15 @@
         <v>32</v>
       </c>
       <c r="H6" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="12"/>
+      <c r="J6" s="11"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>33</v>
       </c>
@@ -797,7 +788,7 @@
         <v>34</v>
       </c>
       <c r="D7" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>15</v>
@@ -809,15 +800,15 @@
         <v>36</v>
       </c>
       <c r="H7" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="12"/>
+      <c r="J7" s="11"/>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>37</v>
       </c>
@@ -840,15 +831,15 @@
         <v>40</v>
       </c>
       <c r="H8" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="12"/>
+      <c r="J8" s="11"/>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>41</v>
       </c>
@@ -859,7 +850,7 @@
         <v>42</v>
       </c>
       <c r="D9" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>15</v>
@@ -871,15 +862,15 @@
         <v>44</v>
       </c>
       <c r="H9" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="12"/>
+      <c r="J9" s="11"/>
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -890,7 +881,7 @@
         <v>46</v>
       </c>
       <c r="D10" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>15</v>
@@ -902,15 +893,15 @@
         <v>48</v>
       </c>
       <c r="H10" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="12"/>
+      <c r="J10" s="11"/>
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>49</v>
       </c>
@@ -921,7 +912,7 @@
         <v>50</v>
       </c>
       <c r="D11" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>22</v>
@@ -933,15 +924,15 @@
         <v>52</v>
       </c>
       <c r="H11" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="12"/>
+      <c r="J11" s="11"/>
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>53</v>
       </c>
@@ -952,7 +943,7 @@
         <v>54</v>
       </c>
       <c r="D12" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>22</v>
@@ -964,12 +955,12 @@
         <v>56</v>
       </c>
       <c r="H12" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="12"/>
+      <c r="J12" s="11"/>
       <c r="K12" s="6"/>
     </row>
   </sheetData>

</xml_diff>